<commit_message>
Fixed variables and query errors in Bread from TC30 to TC47
</commit_message>
<xml_diff>
--- a/InputFiles/TC31_Canine_Filter_Breed-IrishSettr.xlsx
+++ b/InputFiles/TC31_Canine_Filter_Breed-IrishSettr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0D52DB-F49A-4394-9AF0-04540271E163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C093F844-B8C6-4ACF-8DF9-74CC4EB8820A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,47 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE demo.breed IN ['Irish Setter']
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>TC31_Canine_Filter_Breed-IrishSettr_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC31_Canine_Filter_Breed-IrishSettr_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['Irish Setter']
+OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN  coalesce(f.file_name, '') AS `File Name`,
+           coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`,
+         coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 WHERE demo.breed IN ['Irish Setter']
 MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
@@ -76,49 +116,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`
-</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE demo.breed IN ['Irish Setter']
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>TC31_Canine_Filter_Breed-IrishSettr_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC31_Canine_Filter_Breed-IrishSettr_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Irish Setter']
-OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN  coalesce(f.file_name, '') AS `File Name`,
-           coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-         coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
   </si>
 </sst>
 </file>
@@ -490,19 +488,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="44.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.77734375" customWidth="1"/>
+    <col min="4" max="4" width="70.21875" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -519,55 +517,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>